<commit_message>
PDC info toegevoegd aan Grafsoorten per gemeente xlsx
</commit_message>
<xml_diff>
--- a/documenten/Datamodel/Gebruikersonderzoek/Grafsoorten West Friesland per gemeente.xlsx
+++ b/documenten/Datamodel/Gebruikersonderzoek/Grafsoorten West Friesland per gemeente.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hfran\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\VTFD91UJ\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F87D3EA7-3265-4FFF-A51F-B21C2E573F60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="25785" windowHeight="13980" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="SED Gemeentes" sheetId="1" r:id="rId1"/>
@@ -18,8 +12,10 @@
     <sheet name="Gemeente Koggenland" sheetId="3" r:id="rId3"/>
     <sheet name="Gemeente Medemblik" sheetId="4" r:id="rId4"/>
     <sheet name="Gemeente Opmeer" sheetId="5" r:id="rId5"/>
+    <sheet name="Gemeente SED" sheetId="7" r:id="rId6"/>
+    <sheet name="productendienstencatalogues" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="195">
   <si>
     <t>ID</t>
   </si>
@@ -578,12 +574,48 @@
   </si>
   <si>
     <t>Urn</t>
+  </si>
+  <si>
+    <t>Kindergraf</t>
+  </si>
+  <si>
+    <t>Huurgraf</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Zoals in productendienstencatalogues</t>
+  </si>
+  <si>
+    <t>productendienstencatalogues grafsoorten</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Babygraf</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>* = opgesplitst in urnennis en urngraf</t>
+  </si>
+  <si>
+    <t>??? = moet dit wel een graf soort zijn?</t>
+  </si>
+  <si>
+    <t>x = niet aanwezig in het PDC</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -621,10 +653,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -897,27 +932,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5859375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.29296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.5">
@@ -1408,22 +1443,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5859375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="56.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1436,8 +1473,12 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1450,8 +1491,11 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F2" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1464,8 +1508,11 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F3" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1478,8 +1525,11 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1492,8 +1542,11 @@
       <c r="D5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1506,8 +1559,11 @@
       <c r="D6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F6" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1520,8 +1576,11 @@
       <c r="D7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F7" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1534,8 +1593,11 @@
       <c r="D8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F8" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1548,8 +1610,11 @@
       <c r="D9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F9" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1562,8 +1627,11 @@
       <c r="D10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F10" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1576,8 +1644,11 @@
       <c r="D11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F11" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1590,8 +1661,11 @@
       <c r="D12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F12" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1604,8 +1678,11 @@
       <c r="D13" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F13" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1618,8 +1695,11 @@
       <c r="D14" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F14" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1632,8 +1712,11 @@
       <c r="D15" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F15" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1646,8 +1729,11 @@
       <c r="D16" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F16" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1660,8 +1746,11 @@
       <c r="D17" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F17" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1674,8 +1763,11 @@
       <c r="D18" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F18" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1688,8 +1780,11 @@
       <c r="D19" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F19" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1702,8 +1797,11 @@
       <c r="D20" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F20" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1716,8 +1814,11 @@
       <c r="D21" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F21" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1730,8 +1831,11 @@
       <c r="D22" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F22" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1744,8 +1848,11 @@
       <c r="D23" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F23" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1758,8 +1865,11 @@
       <c r="D24" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F24" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1772,8 +1882,11 @@
       <c r="D25" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F25" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1786,8 +1899,11 @@
       <c r="D26" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F26" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1800,8 +1916,11 @@
       <c r="D27" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F27" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1814,8 +1933,11 @@
       <c r="D28" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F28" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1828,8 +1950,11 @@
       <c r="D29" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F29" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1842,8 +1967,11 @@
       <c r="D30" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F30" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1856,8 +1984,11 @@
       <c r="D31" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F31" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1870,8 +2001,11 @@
       <c r="D32" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F32" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1883,6 +2017,14 @@
       </c>
       <c r="D33" t="s">
         <v>149</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -1891,22 +2033,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.87890625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5859375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.87890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1919,8 +2062,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F1" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1933,8 +2079,11 @@
       <c r="D2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F2" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1947,8 +2096,11 @@
       <c r="D3" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F3" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1961,8 +2113,11 @@
       <c r="D4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F4" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1975,8 +2130,11 @@
       <c r="D5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F5" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1989,8 +2147,11 @@
       <c r="D6" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F6" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2003,8 +2164,11 @@
       <c r="D7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F7" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2017,8 +2181,11 @@
       <c r="D8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F8" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2031,8 +2198,11 @@
       <c r="D9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F9" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2045,8 +2215,11 @@
       <c r="D10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F10" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2059,6 +2232,75 @@
       <c r="D11" t="s">
         <v>4</v>
       </c>
+      <c r="F11" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2066,21 +2308,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5859375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.87890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2090,8 +2333,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E1" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2101,8 +2347,11 @@
       <c r="C2" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E2" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2112,19 +2361,22 @@
       <c r="C3" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A4">
-        <v>3</v>
-      </c>
+      <c r="E3" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E4" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2134,8 +2386,11 @@
       <c r="C5" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E5" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2145,8 +2400,11 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2156,8 +2414,11 @@
       <c r="C7" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E7" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2167,8 +2428,11 @@
       <c r="C8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E8" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10</v>
       </c>
@@ -2178,8 +2442,11 @@
       <c r="C9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E9" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>15</v>
       </c>
@@ -2189,8 +2456,11 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20</v>
       </c>
@@ -2200,8 +2470,11 @@
       <c r="C11" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E11" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>22</v>
       </c>
@@ -2211,8 +2484,11 @@
       <c r="C12" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E12" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>23</v>
       </c>
@@ -2222,8 +2498,11 @@
       <c r="C13" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E13" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>24</v>
       </c>
@@ -2233,8 +2512,11 @@
       <c r="C14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E14" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>25</v>
       </c>
@@ -2244,8 +2526,11 @@
       <c r="C15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E15" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>26</v>
       </c>
@@ -2255,8 +2540,11 @@
       <c r="C16" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E16" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>28</v>
       </c>
@@ -2266,8 +2554,11 @@
       <c r="C17" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E17" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>29</v>
       </c>
@@ -2277,6 +2568,58 @@
       <c r="C18" t="s">
         <v>180</v>
       </c>
+      <c r="E18" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2284,21 +2627,175 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.87890625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5859375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5859375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2308,28 +2805,263 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="E1" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" t="s">
+        <v>194</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>182</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>